<commit_message>
added script to calculate the error correction, corrected angles and the sum of the total distance
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -1,99 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\PycharmProjects\traversingComputation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8955" windowHeight="6885"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="14460" windowHeight="8175" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Station</t>
-  </si>
-  <si>
-    <t>Observed Angles</t>
-  </si>
-  <si>
-    <t>Distance</t>
-  </si>
-  <si>
-    <t>Adjustment</t>
-  </si>
-  <si>
-    <t>Adjusted Angles</t>
-  </si>
-  <si>
-    <t>Bearing</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Bearing AF</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,24 +45,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -391,172 +385,154 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col width="14.28515625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Stns</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Obs Angles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Distance</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Corrected Angles</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>W.C.B</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
       </c>
       <c r="B2">
-        <f>(115)+(11/60)+(20/3600)</f>
-        <v>115.1888888888889</v>
-      </c>
-      <c r="C2">
-        <v>85.974000000000004</v>
-      </c>
-      <c r="D2">
-        <v>-2.7777777777777779E-3</v>
-      </c>
-      <c r="E2">
-        <v>115.1861111111111</v>
+        <f>(86)+(30/60)+(2/3600)</f>
+        <v/>
+      </c>
+      <c r="C2" t="n">
+        <v>187.4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.0013888888888971</v>
+      </c>
+      <c r="E2" t="n">
+        <v>86.49916666666665</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
       </c>
       <c r="B3">
-        <f>(95)+(0)+(10/3600)</f>
-        <v>95.00277777777778</v>
-      </c>
-      <c r="C3">
-        <v>131.30799999999999</v>
-      </c>
-      <c r="D3">
-        <v>-2.7777777777777779E-3</v>
-      </c>
-      <c r="E3">
-        <v>95</v>
+        <f>(80)+(59/60)+(34/3600)</f>
+        <v/>
+      </c>
+      <c r="C3" t="n">
+        <v>382.7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.0013888888888971</v>
+      </c>
+      <c r="E3" t="n">
+        <v>80.99138888888888</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
       </c>
       <c r="B4">
-        <f>129+(49/60)+(10/3600)</f>
-        <v>129.81944444444443</v>
-      </c>
-      <c r="C4">
-        <v>60.366999999999997</v>
-      </c>
-      <c r="D4">
-        <v>-2.7777777777777779E-3</v>
-      </c>
-      <c r="E4">
-        <v>129.81666666666669</v>
+        <f>(91)+(31/60)+(29/3600)</f>
+        <v/>
+      </c>
+      <c r="C4" t="n">
+        <v>106.1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.0013888888888971</v>
+      </c>
+      <c r="E4" t="n">
+        <v>91.52333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
       </c>
       <c r="B5">
-        <f>130+(36/60)</f>
-        <v>130.6</v>
-      </c>
-      <c r="C5">
-        <v>57.481999999999999</v>
-      </c>
-      <c r="D5">
-        <v>-2.7777777777777779E-3</v>
-      </c>
-      <c r="E5">
-        <v>130.5972222222222</v>
+        <f>(100)+(59/60)+(15/3600)</f>
+        <v/>
+      </c>
+      <c r="C5" t="n">
+        <v>364.8</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.0013888888888971</v>
+      </c>
+      <c r="E5" t="n">
+        <v>100.9861111111111</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <f>110+(29/60)+(50/3600)</f>
-        <v>110.49722222222222</v>
-      </c>
-      <c r="C6">
-        <v>105.34399999999999</v>
-      </c>
-      <c r="D6">
-        <v>-2.7777777777777779E-3</v>
-      </c>
-      <c r="E6">
-        <v>110.4944444444444</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <f>138+(54/60)+(30/3600)</f>
-        <v>138.90833333333333</v>
-      </c>
-      <c r="C7">
-        <v>74.495999999999995</v>
-      </c>
-      <c r="D7">
-        <v>-2.7777777777777779E-3</v>
-      </c>
-      <c r="E7">
-        <v>138.90555555555559</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2">
-        <v>720.01666666666665</v>
-      </c>
-      <c r="E8" s="2">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1">
-        <v>70</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>360.0055555555556</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1041</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.005555555555588398</v>
+      </c>
+      <c r="E7" t="n">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wrote the script for the bearings,departure and latitude
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="14460" windowHeight="8175" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="8955" windowHeight="6885" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -24,13 +24,24 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor rgb="0071FF33"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -45,8 +56,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,26 +403,31 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14.28515625" customWidth="1" min="2" max="2"/>
+    <col width="16.7109375" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="12.85546875" customWidth="1" min="4" max="4"/>
+    <col width="16.42578125" customWidth="1" min="5" max="5"/>
+    <col width="12.5703125" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Stns</t>
+          <t>Station</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Obs Angles</t>
+          <t>Observed Angles</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -430,6 +448,16 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>W.C.B</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Departure</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Latitude</t>
         </is>
       </c>
     </row>
@@ -440,17 +468,26 @@
         </is>
       </c>
       <c r="B2">
-        <f>(86)+(30/60)+(2/3600)</f>
+        <f>(81)+(11/60)+(50/3600)</f>
         <v/>
       </c>
       <c r="C2" t="n">
-        <v>187.4</v>
+        <v>155</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.0013888888888971</v>
+        <v>0.002777777777782831</v>
       </c>
       <c r="E2" t="n">
-        <v>86.49916666666665</v>
+        <v>81.2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>155</v>
       </c>
     </row>
     <row r="3">
@@ -460,17 +497,26 @@
         </is>
       </c>
       <c r="B3">
-        <f>(80)+(59/60)+(34/3600)</f>
+        <f>(120)+(25/60)+(50/3600)</f>
         <v/>
       </c>
       <c r="C3" t="n">
-        <v>382.7</v>
+        <v>200</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.0013888888888971</v>
+        <v>0.002777777777782831</v>
       </c>
       <c r="E3" t="n">
-        <v>80.99138888888888</v>
+        <v>120.4333333333333</v>
+      </c>
+      <c r="F3" t="n">
+        <v>300.4333333333333</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-172.44</v>
+      </c>
+      <c r="H3" t="n">
+        <v>101.31</v>
       </c>
     </row>
     <row r="4">
@@ -480,17 +526,26 @@
         </is>
       </c>
       <c r="B4">
-        <f>(91)+(31/60)+(29/3600)</f>
+        <f>(149)+(33/60)+(50/3600)</f>
         <v/>
       </c>
       <c r="C4" t="n">
-        <v>106.1</v>
+        <v>249</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0013888888888971</v>
+        <v>0.002777777777782831</v>
       </c>
       <c r="E4" t="n">
-        <v>91.52333333333333</v>
+        <v>149.5666666666667</v>
+      </c>
+      <c r="F4" t="n">
+        <v>270</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-249</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-0</v>
       </c>
     </row>
     <row r="5">
@@ -500,39 +555,90 @@
         </is>
       </c>
       <c r="B5">
-        <f>(100)+(59/60)+(15/3600)</f>
+        <f>95+(41/60)+(50/3600)</f>
         <v/>
       </c>
       <c r="C5" t="n">
-        <v>364.8</v>
+        <v>190</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0013888888888971</v>
+        <v>0.002777777777782831</v>
       </c>
       <c r="E5" t="n">
-        <v>100.9861111111111</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+        <v>95.7</v>
+      </c>
+      <c r="F5" t="n">
+        <v>185.7</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-18.87</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-189.06</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>93+(5/60)+(50/3600)</f>
+        <v/>
+      </c>
+      <c r="C6" t="n">
+        <v>445</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.002777777777782831</v>
+      </c>
+      <c r="E6" t="n">
+        <v>93.09999999999999</v>
+      </c>
+      <c r="F6" t="n">
+        <v>98.80000000000007</v>
+      </c>
+      <c r="G6" t="n">
+        <v>439.76</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-68.08</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>360.0055555555556</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1041</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-0.005555555555588398</v>
-      </c>
-      <c r="E7" t="n">
-        <v>360</v>
-      </c>
+      <c r="B8" t="n">
+        <v>539.9861111111111</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1239</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.01388888888891415</v>
+      </c>
+      <c r="E8" t="n">
+        <v>540</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>5.684341886080801e-14</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-0.5500000000000114</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-0.8299999999999983</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added the errors at the Depature and Latitude for each traverse line
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -403,7 +403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -460,6 +460,16 @@
           <t>Latitude</t>
         </is>
       </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>errorDeparture</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>errorLatitude</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -489,6 +499,12 @@
       <c r="H2" t="n">
         <v>155</v>
       </c>
+      <c r="I2" t="n">
+        <v>0.06880548829701515</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.1038337368845841</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -518,6 +534,12 @@
       <c r="H3" t="n">
         <v>101.31</v>
       </c>
+      <c r="I3" t="n">
+        <v>0.08878127522195502</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.1339790153349472</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -547,6 +569,12 @@
       <c r="H4" t="n">
         <v>-0</v>
       </c>
+      <c r="I4" t="n">
+        <v>0.110532687651334</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.1668038740920093</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -576,6 +604,12 @@
       <c r="H5" t="n">
         <v>-189.06</v>
       </c>
+      <c r="I5" t="n">
+        <v>0.08434221146085727</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.1272800645681999</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -605,6 +639,17 @@
       <c r="H6" t="n">
         <v>-68.08</v>
       </c>
+      <c r="I6" t="n">
+        <v>0.1975383373688499</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.2981033091202576</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="F7" s="2" t="n">
+        <v>5.684341886080801e-14</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -624,14 +669,24 @@
       <c r="E8" t="n">
         <v>540</v>
       </c>
-      <c r="F8" s="2" t="n">
-        <v>5.684341886080801e-14</v>
-      </c>
       <c r="G8" t="n">
         <v>-0.5500000000000114</v>
       </c>
       <c r="H8" t="n">
         <v>-0.8299999999999983</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.5500000000000114</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.8299999999999983</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1 / 1245</t>
+        </is>
       </c>
     </row>
     <row r="10">

</xml_diff>